<commit_message>
Preparation de la publication 210-ballot (#388)
* Preparation publi 210-ballot

* Update sushi-config.yaml 4d832c8747aeb9da9a75e1e188a5d5e6229d20bb
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
+++ b/main/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>2.1.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-29T16:42:45+00:00</t>
+    <t>2025-11-04T09:41:06+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Publication de la release 210 (#398)
* release 210

* Update changes.md 2d344d4e393333715bcb456209b3d948a6146765
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
+++ b/main/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.1.0-ballot</t>
+    <t>2.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-04T14:52:21+00:00</t>
+    <t>2025-12-08T13:48:42+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Préparation release concertation 220 ballot (#404)
* Release 220-ballot

* Update sushi-config.yaml 69c3d116bf1c1b11ace32dd3a1b1789a63a270dc
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
+++ b/main/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.1.0</t>
+    <t>2.2.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-18T17:25:31+00:00</t>
+    <t>2025-12-19T08:32:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Update FHIR release workflow for IG registry push (#403)
* Update FHIR release workflow for IG registry push

* Update publish path in fhir-release workflow c38d81b3164a16c7abf1c9bcfed5fefc9480e4b8
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
+++ b/main/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.2.0-ballot</t>
+    <t>2.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-19T08:32:44+00:00</t>
+    <t>2025-12-19T08:44:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>